<commit_message>
Added new Image Arrays etc
Added image arrays, including masking and histogram shifting. Updated plots for the paper.
</commit_message>
<xml_diff>
--- a/Catalog/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Catalog/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F36D11-E93A-4ECF-A0BC-E57CCA65CEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AEC8EF-AEA9-4B23-B345-E104007FE2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" firstSheet="1" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="133">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -2726,13 +2726,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC165"/>
+  <dimension ref="A1:AC167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B156" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D171" sqref="D171"/>
+      <selection pane="bottomRight" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8720,6 +8720,70 @@
         <v>87</v>
       </c>
       <c r="N165" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A166" s="53">
+        <v>45342</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J166" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K166" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L166" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M166" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N166" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A167" s="53">
+        <v>45342</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H167" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I167" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J167" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K167" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L167" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M167" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N167" s="3" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>